<commit_message>
Update to recent XMMSSC analysis.
</commit_message>
<xml_diff>
--- a/4XMMSSC/dets_to_review.xlsx
+++ b/4XMMSSC/dets_to_review.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/do19150/Gits/ML_QPE/4XMMSSC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{552CEFC3-8549-DA4D-B1BF-D7AC41FD9A18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D16DDA8A-C95A-A643-9EA4-289791EE90A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="880" yWindow="1280" windowWidth="23420" windowHeight="16720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dets_to_review" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="41">
   <si>
     <t>OBSID</t>
   </si>
@@ -75,6 +75,90 @@
   </si>
   <si>
     <t>X-ray source</t>
+  </si>
+  <si>
+    <t>[GY 92] 463</t>
+  </si>
+  <si>
+    <t>T Tauri Star</t>
+  </si>
+  <si>
+    <t>[GY 92] 259</t>
+  </si>
+  <si>
+    <t>YSO</t>
+  </si>
+  <si>
+    <t>V* V1320 Ori</t>
+  </si>
+  <si>
+    <t>BY Dra Variable Star</t>
+  </si>
+  <si>
+    <t>X LMC X-4</t>
+  </si>
+  <si>
+    <t>High Mass XRB</t>
+  </si>
+  <si>
+    <t>GAMA 1943631</t>
+  </si>
+  <si>
+    <t>Galaxy</t>
+  </si>
+  <si>
+    <t>SDSS J020617.04-002300.2</t>
+  </si>
+  <si>
+    <t>2MASS J18094902-2336141</t>
+  </si>
+  <si>
+    <t>Emission Line Star</t>
+  </si>
+  <si>
+    <t>IRAS 20190+3645</t>
+  </si>
+  <si>
+    <t>IR source</t>
+  </si>
+  <si>
+    <t>UCAC4 509-131194</t>
+  </si>
+  <si>
+    <t>High Proper Motion Star</t>
+  </si>
+  <si>
+    <t>J181323.3-325232</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>2MASS J08384128+1959471</t>
+  </si>
+  <si>
+    <t>Eruptive Variable</t>
+  </si>
+  <si>
+    <t>J220310.6-344406</t>
+  </si>
+  <si>
+    <t>J035947.1+353906</t>
+  </si>
+  <si>
+    <t>SDSS J032048.68+003234.0</t>
+  </si>
+  <si>
+    <t>Low Mass Star</t>
+  </si>
+  <si>
+    <t>J124901.5-410131</t>
+  </si>
+  <si>
+    <t>J145916.0+483504</t>
+  </si>
+  <si>
+    <t>[LBX2017] 780</t>
   </si>
 </sst>
 </file>
@@ -217,7 +301,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -395,6 +479,18 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -558,9 +654,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -918,8 +1016,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -927,8 +1025,9 @@
     <col min="1" max="1" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="10.83203125" style="1"/>
+    <col min="4" max="4" width="37.5" style="1" customWidth="1"/>
+    <col min="5" max="5" width="31" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -949,457 +1048,593 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
+      <c r="A2" s="2">
         <v>655050101</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="2">
         <v>11</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="2">
         <v>200287402010079</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
+      <c r="A3" s="2">
         <v>801610101</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="2">
         <v>4</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="2">
         <v>200560203010005</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
+      <c r="A4" s="2">
         <v>501790101</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="2">
         <v>2</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="2">
         <v>200669401010002</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
+      <c r="A5" s="2">
         <v>501790101</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="2">
         <v>15</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="2">
         <v>200669401010075</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
+    <row r="6" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="3">
         <v>652250101</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="3">
         <v>70</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="3">
         <v>200795702010086</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="1">
+      <c r="A7" s="2">
         <v>803990301</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="2">
         <v>4</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="2">
         <v>201068601010017</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="1">
+      <c r="A8" s="2">
         <v>555780601</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8" s="2">
         <v>5</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="2">
         <v>201080604010030</v>
       </c>
+      <c r="D8" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="1">
+      <c r="A9" s="2">
         <v>604960801</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9" s="2">
         <v>3</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="2">
         <v>201080604010030</v>
       </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="1">
+      <c r="A10" s="2">
         <v>604961201</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10" s="2">
         <v>5</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="2">
         <v>201080604010030</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="1">
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+    </row>
+    <row r="11" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="3">
         <v>763120301</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11" s="3">
         <v>6</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="3">
         <v>201092703010096</v>
       </c>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="1">
+      <c r="A12" s="2">
         <v>305540701</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12" s="2">
         <v>14</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12" s="2">
         <v>201111202010026</v>
       </c>
+      <c r="D12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="1">
+      <c r="A13" s="2">
         <v>800030801</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13" s="2">
         <v>23</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13" s="2">
         <v>201111202010026</v>
       </c>
+      <c r="D13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="1">
+      <c r="A14" s="2">
         <v>800031001</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14" s="2">
         <v>3</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14" s="2">
         <v>201111202010048</v>
       </c>
+      <c r="D14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="1">
+      <c r="A15" s="2">
         <v>403200101</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15" s="2">
         <v>85</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15" s="2">
         <v>201125903010151</v>
       </c>
+      <c r="D15" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="1">
+      <c r="A16" s="2">
         <v>142800101</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B16" s="2">
         <v>1</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16" s="2">
         <v>201428001010001</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="1">
+      <c r="D16" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="2">
         <v>743830601</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B17" s="2">
         <v>10</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17" s="2">
         <v>201504706010019</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="1">
+      <c r="D17" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="2">
         <v>821240301</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B18" s="2">
         <v>3</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C18" s="2">
         <v>202010902010004</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="1">
+      <c r="D18" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="2">
         <v>201270101</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B19" s="2">
         <v>28</v>
       </c>
-      <c r="C19" s="1">
+      <c r="C19" s="2">
         <v>202012701010038</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="1">
+      <c r="D19" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="2">
         <v>674050101</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B20" s="2">
         <v>34</v>
       </c>
-      <c r="C20" s="1">
+      <c r="C20" s="2">
         <v>204045402010025</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="1">
+      <c r="D20" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="3">
         <v>550950101</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B21" s="3">
         <v>13</v>
       </c>
-      <c r="C21" s="1">
+      <c r="C21" s="3">
         <v>205509501010012</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="1">
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+    </row>
+    <row r="22" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="3">
         <v>723540301</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B22" s="3">
         <v>20</v>
       </c>
-      <c r="C22" s="1">
+      <c r="C22" s="3">
         <v>205524104010020</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="1">
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+    </row>
+    <row r="23" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="3">
         <v>554680101</v>
       </c>
-      <c r="B23" s="1">
+      <c r="B23" s="3">
         <v>28</v>
       </c>
-      <c r="C23" s="1">
+      <c r="C23" s="3">
         <v>205546801010020</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="1">
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="2">
         <v>600690101</v>
       </c>
-      <c r="B24" s="1">
+      <c r="B24" s="2">
         <v>2</v>
       </c>
-      <c r="C24" s="1">
+      <c r="C24" s="2">
         <v>206006901010002</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="1">
+      <c r="D24" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="2">
         <v>604860201</v>
       </c>
-      <c r="B25" s="1">
+      <c r="B25" s="2">
         <v>5</v>
       </c>
-      <c r="C25" s="1">
+      <c r="C25" s="2">
         <v>206048602010005</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="1">
+      <c r="D25" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="3">
         <v>604860301</v>
       </c>
-      <c r="B26" s="1">
+      <c r="B26" s="3">
         <v>28</v>
       </c>
-      <c r="C26" s="1">
+      <c r="C26" s="3">
         <v>206048602010092</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="1">
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+    </row>
+    <row r="27" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="3">
         <v>692050101</v>
       </c>
-      <c r="B27" s="1">
+      <c r="B27" s="3">
         <v>10</v>
       </c>
-      <c r="C27" s="1">
+      <c r="C27" s="3">
         <v>206920501010010</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" s="1">
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+    </row>
+    <row r="28" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="3">
         <v>760900101</v>
       </c>
-      <c r="B28" s="1">
+      <c r="B28" s="3">
         <v>23</v>
       </c>
-      <c r="C28" s="1">
+      <c r="C28" s="3">
         <v>207206901010055</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" s="1">
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="2">
         <v>721620101</v>
       </c>
-      <c r="B29" s="1">
+      <c r="B29" s="2">
         <v>18</v>
       </c>
-      <c r="C29" s="1">
+      <c r="C29" s="2">
         <v>207216201010018</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" s="1">
+      <c r="D29" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" s="2">
         <v>722360301</v>
       </c>
-      <c r="B30" s="1">
+      <c r="B30" s="2">
         <v>22</v>
       </c>
-      <c r="C30" s="1">
+      <c r="C30" s="2">
         <v>207223603010022</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" s="1">
+      <c r="D30" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="3">
         <v>744400501</v>
       </c>
-      <c r="B31" s="1">
+      <c r="B31" s="3">
         <v>44</v>
       </c>
-      <c r="C31" s="1">
+      <c r="C31" s="3">
         <v>207444005010047</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" s="1">
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" s="2">
         <v>770990101</v>
       </c>
-      <c r="B32" s="1">
+      <c r="B32" s="2">
         <v>8</v>
       </c>
-      <c r="C32" s="1">
+      <c r="C32" s="2">
         <v>207709901010008</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" s="1">
+      <c r="D32" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" s="2">
         <v>781040101</v>
       </c>
-      <c r="B33" s="1">
+      <c r="B33" s="2">
         <v>7</v>
       </c>
-      <c r="C33" s="1">
+      <c r="C33" s="2">
         <v>207810401010007</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" s="1">
+      <c r="D33" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="3">
         <v>801930801</v>
       </c>
-      <c r="B34" s="1">
+      <c r="B34" s="3">
         <v>17</v>
       </c>
-      <c r="C34" s="1">
+      <c r="C34" s="3">
         <v>208019308010017</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" s="1">
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+    </row>
+    <row r="35" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="3">
         <v>822200101</v>
       </c>
-      <c r="B35" s="1">
+      <c r="B35" s="3">
         <v>19</v>
       </c>
-      <c r="C35" s="1">
+      <c r="C35" s="3">
         <v>208222001010019</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" s="1">
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" s="2">
         <v>823580301</v>
       </c>
-      <c r="B36" s="1">
+      <c r="B36" s="2">
         <v>11</v>
       </c>
-      <c r="C36" s="1">
+      <c r="C36" s="2">
         <v>208235803010011</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A37" s="1">
+      <c r="D36" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="3">
         <v>841481701</v>
       </c>
-      <c r="B37" s="1">
+      <c r="B37" s="3">
         <v>23</v>
       </c>
-      <c r="C37" s="1">
+      <c r="C37" s="3">
         <v>208414817010023</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A38" s="1">
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+    </row>
+    <row r="38" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="3">
         <v>842811001</v>
       </c>
-      <c r="B38" s="1">
+      <c r="B38" s="3">
         <v>31</v>
       </c>
-      <c r="C38" s="1">
+      <c r="C38" s="3">
         <v>208428110010031</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A39" s="1">
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" s="2">
         <v>862730501</v>
       </c>
-      <c r="B39" s="1">
+      <c r="B39" s="2">
         <v>6</v>
       </c>
-      <c r="C39" s="1">
+      <c r="C39" s="2">
         <v>208627305010006</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated plots for paper.
</commit_message>
<xml_diff>
--- a/4XMMSSC/dets_to_review.xlsx
+++ b/4XMMSSC/dets_to_review.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/do19150/Gits/ML_QPE/4XMMSSC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D16DDA8A-C95A-A643-9EA4-289791EE90A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84228D51-1CAF-5446-B7CC-520372FAD18E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="880" yWindow="1280" windowWidth="23420" windowHeight="16720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1280" windowWidth="23420" windowHeight="16720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dets_to_review" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="42">
   <si>
     <t>OBSID</t>
   </si>
@@ -159,6 +159,9 @@
   </si>
   <si>
     <t>[LBX2017] 780</t>
+  </si>
+  <si>
+    <t>Low-Mass Star</t>
   </si>
 </sst>
 </file>
@@ -1016,8 +1019,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1112,7 +1115,7 @@
         <v>9</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:5" hidden="1" x14ac:dyDescent="0.2">

</xml_diff>